<commit_message>
added verifications of SSRS PDF and Views to ComplianceReportsPageTest2
</commit_message>
<xml_diff>
--- a/docs/AutomatedTests-ComplianceReports.xlsx
+++ b/docs/AutomatedTests-ComplianceReports.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19608" windowHeight="8208"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19608" windowHeight="8208" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CRPT" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="214">
   <si>
     <t>TestCase</t>
   </si>
@@ -75,9 +75,6 @@
     <t>TC170</t>
   </si>
   <si>
-    <t>Not verified:Report will be generate successfully with same report title but report id will be unique</t>
-  </si>
-  <si>
     <t>TC174</t>
   </si>
   <si>
@@ -189,9 +186,6 @@
     <t>TC1709</t>
   </si>
   <si>
-    <t>Need Verification on SSRS image,View image and ISOTopicAnalysis Table</t>
-  </si>
-  <si>
     <t>TC720</t>
   </si>
   <si>
@@ -201,51 +195,27 @@
     <t>TC824</t>
   </si>
   <si>
-    <t>Not verified: Lisa_Number present in Indications table should be sequential</t>
-  </si>
-  <si>
     <t>TC1038</t>
   </si>
   <si>
     <t xml:space="preserve">TC1041 </t>
   </si>
   <si>
-    <t>Not verified: grid cells should be approximately 200 feet square</t>
-  </si>
-  <si>
     <t>TC1091</t>
   </si>
   <si>
-    <t>Not verified: Views will not show Gaps</t>
-  </si>
-  <si>
     <t>TC1092</t>
   </si>
   <si>
-    <t>Not verified: Views will show Gaps; SSRS will not show Gaps Table</t>
-  </si>
-  <si>
     <t>TC1237</t>
   </si>
   <si>
-    <t>Not verified: View1 has Gaps info, View2 doesn't have gaps info</t>
-  </si>
-  <si>
     <t>TC1257</t>
   </si>
   <si>
-    <t xml:space="preserve">P </t>
-  </si>
-  <si>
-    <t>Not verified: Reference gas capture result and note should not be displayed</t>
-  </si>
-  <si>
     <t>TC1267</t>
   </si>
   <si>
-    <t>Not verified: In Views section, Assets and Boundaries check box is not present; In Optional Views Layers, Assets and Boundaries types are not displayed</t>
-  </si>
-  <si>
     <t>TC1268</t>
   </si>
   <si>
@@ -297,9 +267,6 @@
     <t>TC1090</t>
   </si>
   <si>
-    <t>Not verified: Views will have the Gaps</t>
-  </si>
-  <si>
     <t>TC1319</t>
   </si>
   <si>
@@ -676,6 +643,36 @@
   </si>
   <si>
     <t>Fixed: Not verified:Message should be displayed : 'No matching records found'</t>
+  </si>
+  <si>
+    <t>Fixed: Not verified:Report will be generate successfully with same report title but report id will be unique</t>
+  </si>
+  <si>
+    <t>Fixed: Need Verification on SSRS image,View image and ISOTopicAnalysis Table</t>
+  </si>
+  <si>
+    <t>Fixed: Not verified: Lisa_Number present in Indications table should be sequential</t>
+  </si>
+  <si>
+    <t>Fixed: Not verified: grid cells should be approximately 200 feet square</t>
+  </si>
+  <si>
+    <t>Fixed: Not verified: Views will not show Gaps</t>
+  </si>
+  <si>
+    <t>Fixed: Not verified: Views will show Gaps; SSRS will not show Gaps Table</t>
+  </si>
+  <si>
+    <t>Fixed: Not verified: View1 has Gaps info, View2 doesn't have gaps info</t>
+  </si>
+  <si>
+    <t>Fixed: Not verified: Reference gas capture result and note should not be displayed</t>
+  </si>
+  <si>
+    <t>Fixed: Not verified: In Views section, Assets and Boundaries check box is not present; In Optional Views Layers, Assets and Boundaries types are not displayed</t>
+  </si>
+  <si>
+    <t>Fixed: Not verified: Views will have the Gaps</t>
   </si>
 </sst>
 </file>
@@ -1044,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,7 +1069,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1080,10 +1077,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1091,10 +1088,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1102,7 +1099,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1121,10 +1118,10 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1132,10 +1129,10 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1143,108 +1140,108 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>204</v>
       </c>
       <c r="F9" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
       <c r="F10" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
         <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
         <v>24</v>
-      </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1258,7 +1255,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C10" sqref="C10:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1281,223 +1278,223 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
         <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>205</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1509,8 +1506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1532,227 +1529,227 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -1787,242 +1784,242 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2057,32 +2054,32 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2117,260 +2114,260 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2405,241 +2402,241 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="B26" t="s">
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -2674,169 +2671,169 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed SSRS image verifications from TC1090 and TC1267
</commit_message>
<xml_diff>
--- a/docs/AutomatedTests-ComplianceReports.xlsx
+++ b/docs/AutomatedTests-ComplianceReports.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19608" windowHeight="8208" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19608" windowHeight="8208" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CRPT" sheetId="1" r:id="rId1"/>
@@ -663,16 +663,16 @@
     <t>Fixed: Not verified: Reference gas capture result and note should not be displayed</t>
   </si>
   <si>
-    <t>Fixed: Not verified: In Views section, Assets and Boundaries check box is not present; In Optional Views Layers, Assets and Boundaries types are not displayed</t>
-  </si>
-  <si>
-    <t>Fixed: Not verified: Views will have the Gaps</t>
-  </si>
-  <si>
     <t>Fixed: Depend on US2833</t>
   </si>
   <si>
     <t>Fixed: Depend on DE2003</t>
+  </si>
+  <si>
+    <t>Not verified:Report generated successfully having specified timezone and asset data for specified tag id and date range surveys</t>
+  </si>
+  <si>
+    <t>Not verified: SSRS will have the Gap table. The Gap Table will have numbers corresponding to the gaps in the Compliance View with a check box next to each number. The numbers will run sequentially from left to right and then top to bottom. The numbers in the table should exactly match the number of gaps in the ViewSSRS Gap table should not show Gaps which are completely covered by FoV and LISA</t>
   </si>
 </sst>
 </file>
@@ -1506,8 +1506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1617,10 +1617,10 @@
         <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1746,10 +1746,10 @@
         <v>77</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -1915,7 +1915,7 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -2091,7 +2091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -2334,7 +2334,7 @@
         <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added tests to complianceReportsPageTest4
</commit_message>
<xml_diff>
--- a/docs/AutomatedTests-ComplianceReports.xlsx
+++ b/docs/AutomatedTests-ComplianceReports.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19608" windowHeight="8208" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19608" windowHeight="8208"/>
   </bookViews>
   <sheets>
     <sheet name="CRPT" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="216">
   <si>
     <t>TestCase</t>
   </si>
@@ -676,6 +676,9 @@
   </si>
   <si>
     <t>once the report gets generated, download and check the color of Indication.  There should be default color for Indication.</t>
+  </si>
+  <si>
+    <t>TC154</t>
   </si>
 </sst>
 </file>
@@ -1042,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1069,7 +1072,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>215</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
@@ -1077,125 +1080,125 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>201</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="F8" t="s">
-        <v>195</v>
+      <c r="C8" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
-        <v>202</v>
-      </c>
       <c r="F9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>202</v>
       </c>
       <c r="F10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
         <v>30</v>
@@ -1203,7 +1206,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
         <v>30</v>
@@ -1211,7 +1214,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
         <v>30</v>
@@ -1219,31 +1222,39 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>27</v>
       </c>
-      <c r="B19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1257,7 +1268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated doc - compliancereports.xlsx
</commit_message>
<xml_diff>
--- a/docs/AutomatedTests-ComplianceReports.xlsx
+++ b/docs/AutomatedTests-ComplianceReports.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19608" windowHeight="8208"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19608" windowHeight="8208" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CRPT" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="218">
   <si>
     <t>TestCase</t>
   </si>
@@ -78,18 +78,12 @@
     <t>TC174</t>
   </si>
   <si>
-    <t>Not tested: Rapid Response and Operator Survey modes</t>
-  </si>
-  <si>
     <t>TC181</t>
   </si>
   <si>
     <t>TC184</t>
   </si>
   <si>
-    <t>Not tested: Map selector, and too small area</t>
-  </si>
-  <si>
     <t>TC185</t>
   </si>
   <si>
@@ -438,9 +432,6 @@
     <t>TC180</t>
   </si>
   <si>
-    <t>Not verified: UI should remove surveys other than manual and only manual surveys shows up</t>
-  </si>
-  <si>
     <t>TC182</t>
   </si>
   <si>
@@ -679,6 +670,21 @@
   </si>
   <si>
     <t>TC154</t>
+  </si>
+  <si>
+    <t>Fixed: Not verified: UI should remove surveys other than manual and only manual surveys shows up</t>
+  </si>
+  <si>
+    <t>TC165</t>
+  </si>
+  <si>
+    <t>TC175</t>
+  </si>
+  <si>
+    <t>TC183</t>
+  </si>
+  <si>
+    <t>TC191</t>
   </si>
 </sst>
 </file>
@@ -1047,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,10 +1078,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1083,7 +1089,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1091,10 +1097,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1102,10 +1108,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1113,7 +1119,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1132,10 +1138,10 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1143,10 +1149,10 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1154,13 +1160,13 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1168,94 +1174,88 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1292,226 +1292,226 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -1546,227 +1546,227 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -1801,242 +1801,242 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
         <v>83</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2046,10 +2046,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2071,32 +2071,64 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>135</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2131,260 +2163,260 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2419,241 +2451,241 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
         <v>168</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
         <v>169</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>167</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
         <v>170</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B26" t="s">
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2688,169 +2720,169 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified test data to fix reporting issues
</commit_message>
<xml_diff>
--- a/docs/AutomatedTests-ComplianceReports.xlsx
+++ b/docs/AutomatedTests-ComplianceReports.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="219">
   <si>
     <t>TestCase</t>
   </si>
@@ -685,6 +685,9 @@
   </si>
   <si>
     <t>TC191</t>
+  </si>
+  <si>
+    <t>Need customer other than picarro with assets and surveys available to be tested on SQAAuto</t>
   </si>
 </sst>
 </file>
@@ -2049,7 +2052,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2104,7 +2107,7 @@
         <v>214</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -2112,7 +2115,10 @@
         <v>215</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -2120,7 +2126,7 @@
         <v>216</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -2128,7 +2134,7 @@
         <v>217</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added assets/boundries for SQACUS to test data
</commit_message>
<xml_diff>
--- a/docs/AutomatedTests-ComplianceReports.xlsx
+++ b/docs/AutomatedTests-ComplianceReports.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="218">
   <si>
     <t>TestCase</t>
   </si>
@@ -685,9 +685,6 @@
   </si>
   <si>
     <t>TC191</t>
-  </si>
-  <si>
-    <t>Need customer other than picarro with assets and surveys available to be tested on SQAAuto</t>
   </si>
 </sst>
 </file>
@@ -2052,7 +2049,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2115,10 +2112,7 @@
         <v>215</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>218</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added/Enabled TC207 TC238 in CRPT10
</commit_message>
<xml_diff>
--- a/docs/AutomatedTests-ComplianceReports.xlsx
+++ b/docs/AutomatedTests-ComplianceReports.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19608" windowHeight="8208" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19608" windowHeight="8208" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="CRPT" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="CRPT_5" sheetId="6" r:id="rId6"/>
     <sheet name="CRPT_6" sheetId="7" r:id="rId7"/>
     <sheet name="CRPT_8" sheetId="8" r:id="rId8"/>
+    <sheet name="CRPT10" sheetId="9" r:id="rId9"/>
+    <sheet name="AssetBox" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="226">
   <si>
     <t>TestCase</t>
   </si>
@@ -685,6 +687,30 @@
   </si>
   <si>
     <t>TC191</t>
+  </si>
+  <si>
+    <t>Fixed - Required: CusSupervisor with assets</t>
+  </si>
+  <si>
+    <t>TC207</t>
+  </si>
+  <si>
+    <t>TC238</t>
+  </si>
+  <si>
+    <t>TC2197</t>
+  </si>
+  <si>
+    <t>TC2198</t>
+  </si>
+  <si>
+    <t>TC2199</t>
+  </si>
+  <si>
+    <t>TC2200</t>
+  </si>
+  <si>
+    <t>TC927</t>
   </si>
 </sst>
 </file>
@@ -1264,6 +1290,77 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="3" max="3" width="30.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
@@ -1521,10 +1618,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1767,6 +1864,14 @@
       </c>
       <c r="C25" t="s">
         <v>210</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2048,7 +2153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -2141,7 +2246,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2292,10 +2397,10 @@
         <v>149</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>146</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -2698,7 +2803,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2814,10 +2919,7 @@
         <v>120</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>121</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -2883,6 +2985,50 @@
       </c>
       <c r="B20" t="s">
         <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="39.109375" customWidth="1"/>
+    <col min="3" max="3" width="57.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added CRPT8 to local branch test
</commit_message>
<xml_diff>
--- a/docs/AutomatedTests-ComplianceReports.xlsx
+++ b/docs/AutomatedTests-ComplianceReports.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19608" windowHeight="8208" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19608" windowHeight="8208" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="CRPT" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="227">
   <si>
     <t>TestCase</t>
   </si>
@@ -711,6 +711,9 @@
   </si>
   <si>
     <t>TC927</t>
+  </si>
+  <si>
+    <t>Fixed - Required: CusAdmin</t>
   </si>
 </sst>
 </file>
@@ -1294,7 +1297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -2802,8 +2805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2844,10 +2847,10 @@
         <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated tag name in SurveyorConstants
</commit_message>
<xml_diff>
--- a/docs/AutomatedTests-ComplianceReports.xlsx
+++ b/docs/AutomatedTests-ComplianceReports.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\surveyor-qa\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxiang\dev\surveyor-qa\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19608" windowHeight="8208"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19608" windowHeight="8208" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="CRPT" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="234">
   <si>
     <t>TestCase</t>
   </si>
@@ -731,6 +731,12 @@
   </si>
   <si>
     <t>TC1314</t>
+  </si>
+  <si>
+    <t>TC194</t>
+  </si>
+  <si>
+    <t>Need survey equals 100 hours  - US3885</t>
   </si>
 </sst>
 </file>
@@ -1099,7 +1105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -1309,10 +1315,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1368,6 +1374,17 @@
       </c>
       <c r="B6" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>232</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>